<commit_message>
Generated plots, models and statistics.
</commit_message>
<xml_diff>
--- a/model/results.xlsx
+++ b/model/results.xlsx
@@ -468,10 +468,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>52.13946256889122</v>
+        <v>52.13946256887639</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4971469653529536</v>
+        <v>0.4971469653530965</v>
       </c>
     </row>
     <row r="3">
@@ -486,10 +486,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>163107388553.526</v>
+        <v>163107388526.8221</v>
       </c>
       <c r="D3" t="n">
-        <v>-1573070400.313107</v>
+        <v>-1573070400.055565</v>
       </c>
     </row>
     <row r="4">
@@ -504,16 +504,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>52.69431792143781</v>
+        <v>53.89935221717534</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4917957268845947</v>
+        <v>0.4801739125694827</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Bayes Ridge Regression</t>
+          <t>Lasso Regression with positive Coefficients</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -522,10 +522,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>57.74745449581898</v>
+        <v>73.95363565634419</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4430613338601905</v>
+        <v>0.2867626883603009</v>
       </c>
     </row>
     <row r="6">
@@ -540,10 +540,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>28.72412420860031</v>
+        <v>23.98751883576024</v>
       </c>
       <c r="D6" t="n">
-        <v>0.7229734961922811</v>
+        <v>0.7686551405420108</v>
       </c>
     </row>
     <row r="7">
@@ -558,10 +558,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>14.05235973724497</v>
+        <v>14.2444248244857</v>
       </c>
       <c r="D7" t="n">
-        <v>0.864473636864035</v>
+        <v>0.8626212872767882</v>
       </c>
     </row>
     <row r="8">
@@ -576,10 +576,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>40.48221847609098</v>
+        <v>42.85226970232395</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6095739118321338</v>
+        <v>0.5867162260666638</v>
       </c>
     </row>
     <row r="9">
@@ -594,10 +594,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>91.03617693129569</v>
+        <v>91.03617693129489</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1875999591520345</v>
+        <v>0.1875999591520416</v>
       </c>
     </row>
     <row r="10">
@@ -612,10 +612,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2749121275291.174</v>
+        <v>2749121268259.972</v>
       </c>
       <c r="D10" t="n">
-        <v>-24532952849.47042</v>
+        <v>-24532952786.7245</v>
       </c>
     </row>
     <row r="11">
@@ -630,16 +630,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>92.20453826371266</v>
+        <v>91.95489924413481</v>
       </c>
       <c r="D11" t="n">
-        <v>0.177173589919756</v>
+        <v>0.1794013498778146</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Bayes Ridge Regression</t>
+          <t>Lasso Regression with positive Coefficients</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>99.42852738495505</v>
+        <v>99.68091203694125</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1127072507674464</v>
+        <v>0.1104549889909251</v>
       </c>
     </row>
     <row r="13">
@@ -666,10 +666,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>88.66990383695645</v>
+        <v>92.89837300804287</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2087164034415331</v>
+        <v>0.1709818605036471</v>
       </c>
     </row>
     <row r="14">
@@ -684,10 +684,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>47.08052704443973</v>
+        <v>47.29551685833902</v>
       </c>
       <c r="D14" t="n">
-        <v>0.5798568944419511</v>
+        <v>0.5779383414064311</v>
       </c>
     </row>
     <row r="15">
@@ -702,10 +702,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>80.28883429958134</v>
+        <v>75.67969437911121</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2835084417720939</v>
+        <v>0.3246400620343314</v>
       </c>
     </row>
     <row r="16">
@@ -720,10 +720,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>69.48906955627477</v>
+        <v>69.48906955627709</v>
       </c>
       <c r="D16" t="n">
-        <v>0.4187810453552879</v>
+        <v>0.4187810453552685</v>
       </c>
     </row>
     <row r="17">
@@ -738,10 +738,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>465674854270.5415</v>
+        <v>465674854319.1072</v>
       </c>
       <c r="D17" t="n">
-        <v>-3894987422.658957</v>
+        <v>-3894987423.06517</v>
       </c>
     </row>
     <row r="18">
@@ -756,16 +756,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>71.52202465695994</v>
+        <v>70.52409416323501</v>
       </c>
       <c r="D18" t="n">
-        <v>0.401777046798321</v>
+        <v>0.4101239151917907</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Bayes Ridge Regression</t>
+          <t>Lasso Regression with positive Coefficients</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -774,10 +774,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>83.04373036850707</v>
+        <v>108.0457870943962</v>
       </c>
       <c r="D19" t="n">
-        <v>0.3054074480664477</v>
+        <v>0.09628579243079727</v>
       </c>
     </row>
     <row r="20">
@@ -792,10 +792,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>51.52178681548222</v>
+        <v>47.54066055924312</v>
       </c>
       <c r="D20" t="n">
-        <v>0.5690625983979916</v>
+        <v>0.6023614474937622</v>
       </c>
     </row>
     <row r="21">
@@ -810,10 +810,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>29.0742790629569</v>
+        <v>29.49500624111414</v>
       </c>
       <c r="D21" t="n">
-        <v>0.7568175514231714</v>
+        <v>0.7532985143682698</v>
       </c>
     </row>
     <row r="22">
@@ -828,10 +828,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>59.29902291249969</v>
+        <v>55.80950074928899</v>
       </c>
       <c r="D22" t="n">
-        <v>0.5040124104591108</v>
+        <v>0.5331993953599288</v>
       </c>
     </row>
     <row r="23">
@@ -846,10 +846,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>29.36788088280979</v>
+        <v>29.36788088280915</v>
       </c>
       <c r="D23" t="n">
-        <v>0.5250734874983205</v>
+        <v>0.5250734874983307</v>
       </c>
     </row>
     <row r="24">
@@ -864,10 +864,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2319302743.420866</v>
+        <v>2319302743.494648</v>
       </c>
       <c r="D24" t="n">
-        <v>-37506905.53383853</v>
+        <v>-37506905.53503171</v>
       </c>
     </row>
     <row r="25">
@@ -882,16 +882,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>28.87204493535977</v>
+        <v>30.27669265763229</v>
       </c>
       <c r="D25" t="n">
-        <v>0.5330919631328099</v>
+        <v>0.5103765194583296</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Bayes Ridge Regression</t>
+          <t>Lasso Regression with positive Coefficients</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -900,10 +900,10 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>34.62185970018182</v>
+        <v>53.74202139753132</v>
       </c>
       <c r="D26" t="n">
-        <v>0.4401080844292563</v>
+        <v>0.130903898072532</v>
       </c>
     </row>
     <row r="27">
@@ -918,10 +918,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>26.49065122328525</v>
+        <v>27.62767539645994</v>
       </c>
       <c r="D27" t="n">
-        <v>0.5716029818570447</v>
+        <v>0.5532154472797014</v>
       </c>
     </row>
     <row r="28">
@@ -936,10 +936,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>13.1500100001429</v>
+        <v>11.60238164041661</v>
       </c>
       <c r="D28" t="n">
-        <v>0.7873428997600674</v>
+        <v>0.8123705734443384</v>
       </c>
     </row>
     <row r="29">
@@ -954,10 +954,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>22.43993046133692</v>
+        <v>27.95411761370189</v>
       </c>
       <c r="D29" t="n">
-        <v>0.6371097404913164</v>
+        <v>0.5479363444262577</v>
       </c>
     </row>
     <row r="30">
@@ -972,10 +972,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>38.43626758216376</v>
+        <v>38.43626758216009</v>
       </c>
       <c r="D30" t="n">
-        <v>0.4382436275045052</v>
+        <v>0.4382436275045587</v>
       </c>
     </row>
     <row r="31">
@@ -990,10 +990,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>91993686021.73088</v>
+        <v>91993686026.33995</v>
       </c>
       <c r="D31" t="n">
-        <v>-1344512424.447837</v>
+        <v>-1344512424.515199</v>
       </c>
     </row>
     <row r="32">
@@ -1008,16 +1008,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>39.40337729917719</v>
+        <v>38.88037443180772</v>
       </c>
       <c r="D32" t="n">
-        <v>0.4241090592800214</v>
+        <v>0.4317528866352704</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Bayes Ridge Regression</t>
+          <t>Lasso Regression with positive Coefficients</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1026,10 +1026,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>39.18136178601431</v>
+        <v>67.0402920782105</v>
       </c>
       <c r="D33" t="n">
-        <v>0.4273538756255602</v>
+        <v>0.02018812809050807</v>
       </c>
     </row>
     <row r="34">
@@ -1044,10 +1044,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>31.04172541567423</v>
+        <v>28.60817844625111</v>
       </c>
       <c r="D34" t="n">
-        <v>0.5463168470186641</v>
+        <v>0.5818837894882529</v>
       </c>
     </row>
     <row r="35">
@@ -1062,10 +1062,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>11.82241852906183</v>
+        <v>11.6772285141512</v>
       </c>
       <c r="D35" t="n">
-        <v>0.8272121783726164</v>
+        <v>0.8293341694302656</v>
       </c>
     </row>
     <row r="36">
@@ -1080,10 +1080,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>44.70366092464545</v>
+        <v>46.30263178075999</v>
       </c>
       <c r="D36" t="n">
-        <v>0.3466439907409001</v>
+        <v>0.3232746022867063</v>
       </c>
     </row>
   </sheetData>

</xml_diff>